<commit_message>
Agregado caso prueba 1
</commit_message>
<xml_diff>
--- a/TPO - TEST CASES.xlsx
+++ b/TPO - TEST CASES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Documents/GitHub/TestingAplicaciones-BeSharps-TPO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2725BF91-98AC-004C-9CBA-066A57F7C05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BD6DFD-829F-9F48-A7FA-6F6498909CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15820" xr2:uid="{0C5A14B1-A872-984E-8AE3-DAD24329B4D3}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{0C5A14B1-A872-984E-8AE3-DAD24329B4D3}"/>
   </bookViews>
   <sheets>
     <sheet name="PE-16" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="63">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -153,6 +153,78 @@
   </si>
   <si>
     <t>Acceso a Google Chrome</t>
+  </si>
+  <si>
+    <t>PE-16</t>
+  </si>
+  <si>
+    <t>Usuario ingresa su correo en el campo</t>
+  </si>
+  <si>
+    <t>Usuario cliquea "Register"</t>
+  </si>
+  <si>
+    <t>El sitio se abre</t>
+  </si>
+  <si>
+    <t>Los datos puede ser ingresados</t>
+  </si>
+  <si>
+    <t>El usuario es enviado al formulario</t>
+  </si>
+  <si>
+    <t>Usuario rellena los campos obligatorios con datos correctos</t>
+  </si>
+  <si>
+    <t>Los datos pueden ser ingresados</t>
+  </si>
+  <si>
+    <t>El sistema registra los datos y guarda la cuenta</t>
+  </si>
+  <si>
+    <t>Verificar que el usuario pueda registrar una cuenta con un correo inexistente</t>
+  </si>
+  <si>
+    <t>First Name = Julian</t>
+  </si>
+  <si>
+    <t>Last Name = Alvarez</t>
+  </si>
+  <si>
+    <t>Password = Algo12!</t>
+  </si>
+  <si>
+    <t>City = Miami</t>
+  </si>
+  <si>
+    <t>Email = correo.prueba@exampe.co.uk</t>
+  </si>
+  <si>
+    <t>State = Florida</t>
+  </si>
+  <si>
+    <t>Country = United States</t>
+  </si>
+  <si>
+    <t>Postal Code = 33125</t>
+  </si>
+  <si>
+    <t>Address = 1835 NW 11th St</t>
+  </si>
+  <si>
+    <t>Phone = +1 305-434-9600</t>
+  </si>
+  <si>
+    <t>Date Of Birth = 12/05/1990</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>Navegar a https://sitio.tpo.com/register</t>
   </si>
 </sst>
 </file>
@@ -473,12 +545,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -522,9 +588,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -534,9 +639,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -546,21 +648,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -572,21 +659,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -904,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3EEAB0-B2CC-534D-ADE1-1C36E80F1098}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:AM34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,9 +990,21 @@
     <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="8" max="8" width="22.5" customWidth="1"/>
     <col min="9" max="11" width="14.83203125" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="15" max="15" width="22.5" customWidth="1"/>
+    <col min="16" max="18" width="14.83203125" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" customWidth="1"/>
+    <col min="22" max="22" width="22.5" customWidth="1"/>
+    <col min="23" max="25" width="14.83203125" customWidth="1"/>
+    <col min="28" max="28" width="14.83203125" customWidth="1"/>
+    <col min="29" max="29" width="22.5" customWidth="1"/>
+    <col min="30" max="32" width="14.83203125" customWidth="1"/>
+    <col min="35" max="35" width="14.83203125" customWidth="1"/>
+    <col min="36" max="36" width="22.5" customWidth="1"/>
+    <col min="37" max="39" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,10 +1014,10 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="30"/>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,22 +1027,74 @@
       <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K1" s="30"/>
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="30"/>
+      <c r="U1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="30"/>
+      <c r="AB1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="30"/>
+      <c r="AI1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM1" s="30"/>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -967,363 +1103,1206 @@
       <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="N2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="7">
         <v>2.1</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="N3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="O3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11" t="s">
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="9">
+      <c r="R3" s="7">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="U3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="8"/>
+      <c r="X3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="G5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="G5" s="12" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="N5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="O5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="U5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="AB5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AI5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="18">
+      <c r="N7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM7" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="36" x14ac:dyDescent="0.2">
+      <c r="A8" s="16">
         <v>1</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <v>1</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="18">
+        <v>1</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="18">
+      <c r="N8" s="16">
         <v>1</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="O8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="20">
+      <c r="Q8" s="18">
         <v>1</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="R8" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="18">
+      <c r="U8" s="16">
+        <v>1</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="X8" s="18">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB8" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE8" s="18">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI8" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL8" s="18">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A9" s="16">
         <v>2</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="18">
         <v>2</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="16">
+        <v>2</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="J9" s="18">
+        <v>2</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="18">
+      <c r="N9" s="16">
         <v>2</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="J9" s="20">
+      <c r="O9" s="17"/>
+      <c r="Q9" s="18">
         <v>2</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="R9" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="18">
+      <c r="U9" s="16">
+        <v>2</v>
+      </c>
+      <c r="V9" s="17"/>
+      <c r="X9" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB9" s="16">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="17"/>
+      <c r="AE9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI9" s="16">
+        <v>2</v>
+      </c>
+      <c r="AJ9" s="17"/>
+      <c r="AL9" s="18">
+        <v>2</v>
+      </c>
+      <c r="AM9" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
         <v>3</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="D10" s="20">
+      <c r="B10" s="17"/>
+      <c r="D10" s="18">
         <v>3</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="G10" s="18">
+      <c r="E10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="16">
         <v>3</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="J10" s="20">
+      <c r="H10" s="17"/>
+      <c r="J10" s="18">
         <v>3</v>
       </c>
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="18">
+      <c r="K10" s="17"/>
+      <c r="N10" s="16">
+        <v>3</v>
+      </c>
+      <c r="O10" s="17"/>
+      <c r="Q10" s="18">
+        <v>3</v>
+      </c>
+      <c r="R10" s="17"/>
+      <c r="U10" s="16">
+        <v>3</v>
+      </c>
+      <c r="V10" s="17"/>
+      <c r="X10" s="18">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="17"/>
+      <c r="AB10" s="16">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="17"/>
+      <c r="AE10" s="18">
+        <v>3</v>
+      </c>
+      <c r="AF10" s="17"/>
+      <c r="AI10" s="16">
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="17"/>
+      <c r="AL10" s="18">
+        <v>3</v>
+      </c>
+      <c r="AM10" s="17"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
         <v>4</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="G11" s="18">
+      <c r="B11" s="17"/>
+      <c r="D11" s="18">
         <v>4</v>
       </c>
-      <c r="H11" s="19"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="E11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="16">
+        <v>4</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="N11" s="16">
+        <v>4</v>
+      </c>
+      <c r="O11" s="17"/>
+      <c r="U11" s="16">
+        <v>4</v>
+      </c>
+      <c r="V11" s="17"/>
+      <c r="AB11" s="16">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="17"/>
+      <c r="AI11" s="16">
+        <v>4</v>
+      </c>
+      <c r="AJ11" s="17"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D12" s="18">
+        <v>5</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D13" s="18">
+        <v>6</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="H13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="G13" s="21" t="s">
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="35"/>
+      <c r="N13" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="O13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
-    </row>
-    <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="35"/>
+      <c r="U13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="V13" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="W13" s="34"/>
+      <c r="X13" s="34"/>
+      <c r="Y13" s="35"/>
+      <c r="AB13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC13" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD13" s="34"/>
+      <c r="AE13" s="34"/>
+      <c r="AF13" s="35"/>
+      <c r="AI13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ13" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK13" s="34"/>
+      <c r="AL13" s="34"/>
+      <c r="AM13" s="35"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D14" s="18">
+        <v>7</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="32"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="38"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="38"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="36"/>
+      <c r="AD14" s="37"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="38"/>
+      <c r="AI14" s="32"/>
+      <c r="AJ14" s="36"/>
+      <c r="AK14" s="37"/>
+      <c r="AL14" s="37"/>
+      <c r="AM14" s="38"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D15" s="18">
+        <v>8</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="H15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="29" t="s">
+      <c r="I15" s="21"/>
+      <c r="J15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="K15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="N15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="O15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="31"/>
-      <c r="J15" s="29" t="s">
+      <c r="P15" s="21"/>
+      <c r="Q15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="R15" s="22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="U15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="V15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" s="21"/>
+      <c r="X15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y15" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD15" s="21"/>
+      <c r="AE15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF15" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK15" s="21"/>
+      <c r="AL15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM15" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D16" s="18">
+        <v>9</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D17" s="18">
+        <v>10</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="H17" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36" t="s">
+      <c r="I17" s="40"/>
+      <c r="J17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="G17" s="33" t="s">
+      <c r="K17" s="42"/>
+      <c r="N17" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="O17" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="35"/>
-      <c r="J17" s="36" t="s">
+      <c r="P17" s="40"/>
+      <c r="Q17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="37"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="38">
+      <c r="R17" s="42"/>
+      <c r="U17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="V17" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="W17" s="40"/>
+      <c r="X17" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y17" s="42"/>
+      <c r="AB17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC17" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD17" s="40"/>
+      <c r="AE17" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF17" s="42"/>
+      <c r="AI17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ17" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK17" s="40"/>
+      <c r="AL17" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM17" s="42"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D18" s="18">
+        <v>11</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="24">
         <v>1</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="H18" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="39" t="s">
+      <c r="I18" s="26"/>
+      <c r="J18" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="G18" s="38">
+      <c r="K18" s="26"/>
+      <c r="N18" s="24">
         <v>1</v>
       </c>
-      <c r="H18" s="39" t="s">
+      <c r="O18" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="39" t="s">
+      <c r="P18" s="26"/>
+      <c r="Q18" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="40"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="38">
+      <c r="R18" s="26"/>
+      <c r="U18" s="24">
+        <v>1</v>
+      </c>
+      <c r="V18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="W18" s="26"/>
+      <c r="X18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y18" s="26"/>
+      <c r="AB18" s="24">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD18" s="26"/>
+      <c r="AE18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF18" s="26"/>
+      <c r="AI18" s="24">
+        <v>1</v>
+      </c>
+      <c r="AJ18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK18" s="26"/>
+      <c r="AL18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM18" s="26"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="G19" s="24">
         <v>2</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="H19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="39" t="s">
+      <c r="I19" s="26"/>
+      <c r="J19" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="G19" s="38">
+      <c r="K19" s="26"/>
+      <c r="N19" s="24">
         <v>2</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="O19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="39" t="s">
+      <c r="P19" s="26"/>
+      <c r="Q19" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="40"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="38">
+      <c r="R19" s="26"/>
+      <c r="U19" s="24">
+        <v>2</v>
+      </c>
+      <c r="V19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="W19" s="26"/>
+      <c r="X19" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y19" s="26"/>
+      <c r="AB19" s="24">
+        <v>2</v>
+      </c>
+      <c r="AC19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD19" s="26"/>
+      <c r="AE19" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF19" s="26"/>
+      <c r="AI19" s="24">
+        <v>2</v>
+      </c>
+      <c r="AJ19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM19" s="26"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="G20" s="24">
         <v>3</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="H20" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="39" t="s">
+      <c r="I20" s="26"/>
+      <c r="J20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="G20" s="38">
+      <c r="K20" s="26"/>
+      <c r="N20" s="24">
         <v>3</v>
       </c>
-      <c r="H20" s="39" t="s">
+      <c r="O20" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="40"/>
-      <c r="J20" s="39" t="s">
+      <c r="P20" s="26"/>
+      <c r="Q20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="40"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="38">
+      <c r="R20" s="26"/>
+      <c r="U20" s="24">
+        <v>3</v>
+      </c>
+      <c r="V20" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="W20" s="26"/>
+      <c r="X20" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y20" s="26"/>
+      <c r="AB20" s="24">
+        <v>3</v>
+      </c>
+      <c r="AC20" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD20" s="26"/>
+      <c r="AE20" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF20" s="26"/>
+      <c r="AI20" s="24">
+        <v>3</v>
+      </c>
+      <c r="AJ20" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK20" s="26"/>
+      <c r="AL20" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM20" s="26"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="G21" s="24">
         <v>4</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="G21" s="38">
+      <c r="H21" s="25"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
+      <c r="N21" s="24">
         <v>4</v>
       </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="40"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="40"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="40"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="26"/>
+      <c r="U21" s="24">
+        <v>4</v>
+      </c>
+      <c r="V21" s="25"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="25"/>
+      <c r="Y21" s="26"/>
+      <c r="AB21" s="24">
+        <v>4</v>
+      </c>
+      <c r="AC21" s="25"/>
+      <c r="AD21" s="26"/>
+      <c r="AE21" s="25"/>
+      <c r="AF21" s="26"/>
+      <c r="AI21" s="24">
+        <v>4</v>
+      </c>
+      <c r="AJ21" s="25"/>
+      <c r="AK21" s="26"/>
+      <c r="AL21" s="25"/>
+      <c r="AM21" s="26"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="G22" s="24"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="26"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="25"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="25"/>
+      <c r="Y22" s="26"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="25"/>
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="25"/>
+      <c r="AF22" s="26"/>
+      <c r="AI22" s="24"/>
+      <c r="AJ22" s="25"/>
+      <c r="AK22" s="26"/>
+      <c r="AL22" s="25"/>
+      <c r="AM22" s="26"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="G23" s="24"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="26"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="26"/>
+      <c r="AB23" s="24"/>
+      <c r="AC23" s="25"/>
+      <c r="AD23" s="26"/>
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="26"/>
+      <c r="AI23" s="24"/>
+      <c r="AJ23" s="25"/>
+      <c r="AK23" s="26"/>
+      <c r="AL23" s="25"/>
+      <c r="AM23" s="26"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A24" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A25" s="32"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="42"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A29" s="24">
+        <v>1</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A30" s="24">
+        <v>2</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A31" s="24">
+        <v>3</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A32" s="24">
+        <v>4</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="24">
+        <v>5</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="26"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="103">
+    <mergeCell ref="AJ21:AK21"/>
+    <mergeCell ref="AL21:AM21"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AJ23:AK23"/>
+    <mergeCell ref="AL23:AM23"/>
+    <mergeCell ref="AJ18:AK18"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AJ19:AK19"/>
+    <mergeCell ref="AL19:AM19"/>
+    <mergeCell ref="AJ20:AK20"/>
+    <mergeCell ref="AL20:AM20"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AI13:AI14"/>
+    <mergeCell ref="AJ13:AM14"/>
+    <mergeCell ref="AJ17:AK17"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AF14"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AE17:AF17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="AE22:AF22"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AE19:AF19"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AE20:AF20"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:Y14"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:R14"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:E25"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:K14"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="H23:I23"/>
@@ -1336,30 +2315,12 @@
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:K14"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:E14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>